<commit_message>
Add new scroll bar and new style
</commit_message>
<xml_diff>
--- a/layerInventory.xlsx
+++ b/layerInventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="featureSource" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="169">
   <si>
     <t>mapID</t>
   </si>
@@ -462,9 +462,6 @@
   </si>
   <si>
     <t>wshd_cso</t>
-  </si>
-  <si>
-    <t>wshd_npdes</t>
   </si>
   <si>
     <t>wshd_wshd</t>
@@ -869,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,16 +893,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F1" t="s">
         <v>95</v>
       </c>
       <c r="G1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H1" t="s">
         <v>109</v>
@@ -922,13 +919,13 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -937,7 +934,7 @@
         <v>132</v>
       </c>
       <c r="G2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H2" t="s">
         <v>115</v>
@@ -954,13 +951,13 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -969,7 +966,7 @@
         <v>132</v>
       </c>
       <c r="G3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H3" t="s">
         <v>115</v>
@@ -986,13 +983,13 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -1010,7 +1007,7 @@
         <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1018,13 +1015,13 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -1042,7 +1039,7 @@
         <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1056,16 +1053,16 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H6" t="s">
         <v>135</v>
@@ -1074,7 +1071,7 @@
         <v>110</v>
       </c>
       <c r="J6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1088,7 +1085,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -1097,7 +1094,7 @@
         <v>136</v>
       </c>
       <c r="G7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H7" t="s">
         <v>115</v>
@@ -1126,7 +1123,7 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G8" t="s">
         <v>97</v>
@@ -1149,7 +1146,7 @@
         <v>147</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>135</v>
@@ -1158,42 +1155,42 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
       <c r="G9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I9" t="s">
         <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
         <v>148</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>96</v>
-      </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="H10" t="s">
         <v>114</v>
@@ -1202,7 +1199,7 @@
         <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1210,7 +1207,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -1222,7 +1219,7 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G11" t="s">
         <v>145</v>
@@ -1242,7 +1239,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1254,7 +1251,7 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G12" t="s">
         <v>145</v>
@@ -1274,7 +1271,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1286,7 +1283,7 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G13" t="s">
         <v>145</v>
@@ -1306,7 +1303,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -1318,7 +1315,7 @@
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G14" t="s">
         <v>145</v>
@@ -1335,13 +1332,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
         <v>135</v>
@@ -1350,19 +1347,19 @@
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="H15" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="I15" t="s">
         <v>23</v>
       </c>
       <c r="J15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1370,7 +1367,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -1394,15 +1391,15 @@
         <v>23</v>
       </c>
       <c r="J16" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -1414,83 +1411,83 @@
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="G17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="I17" t="s">
         <v>23</v>
       </c>
       <c r="J17" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="G18" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="H18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I18" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="J18" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="G19" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="H19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I19" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="J19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1498,7 +1495,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1513,7 +1510,7 @@
         <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H20" t="s">
         <v>134</v>
@@ -1530,7 +1527,7 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -1542,7 +1539,7 @@
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="G21" t="s">
         <v>97</v>
@@ -1554,15 +1551,15 @@
         <v>23</v>
       </c>
       <c r="J21" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -1580,13 +1577,13 @@
         <v>97</v>
       </c>
       <c r="H22" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="I22" t="s">
         <v>23</v>
       </c>
       <c r="J22" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1594,7 +1591,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -1618,7 +1615,7 @@
         <v>23</v>
       </c>
       <c r="J23" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1626,10 +1623,10 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
         <v>135</v>
@@ -1638,83 +1635,83 @@
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="G24" t="s">
         <v>97</v>
       </c>
       <c r="H24" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I24" t="s">
         <v>23</v>
       </c>
       <c r="J24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="G25" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="H25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J25" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="E26" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="G26" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="H26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1722,7 +1719,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1746,7 +1743,7 @@
         <v>23</v>
       </c>
       <c r="J27" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1754,7 +1751,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -1778,7 +1775,7 @@
         <v>23</v>
       </c>
       <c r="J28" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1786,7 +1783,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -1810,7 +1807,7 @@
         <v>23</v>
       </c>
       <c r="J29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1818,7 +1815,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -1842,7 +1839,7 @@
         <v>23</v>
       </c>
       <c r="J30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1850,7 +1847,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -1874,7 +1871,7 @@
         <v>23</v>
       </c>
       <c r="J31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1882,7 +1879,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -1906,7 +1903,7 @@
         <v>23</v>
       </c>
       <c r="J32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1914,7 +1911,7 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -1938,7 +1935,7 @@
         <v>23</v>
       </c>
       <c r="J33" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1946,7 +1943,7 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -1970,15 +1967,15 @@
         <v>23</v>
       </c>
       <c r="J34" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -1990,90 +1987,57 @@
         <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G35" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I35" t="s">
         <v>23</v>
       </c>
       <c r="J35" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>167</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" t="s">
-        <v>99</v>
-      </c>
-      <c r="G36" t="s">
-        <v>98</v>
-      </c>
-      <c r="H36" t="s">
-        <v>114</v>
-      </c>
-      <c r="I36" t="s">
-        <v>23</v>
-      </c>
-      <c r="J36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>167</v>
-      </c>
-      <c r="B37" t="s">
         <v>168</v>
-      </c>
-      <c r="C37" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J36" r:id="rId2"/>
-    <hyperlink ref="J29" r:id="rId3"/>
-    <hyperlink ref="J30" r:id="rId4"/>
-    <hyperlink ref="J31" r:id="rId5"/>
-    <hyperlink ref="J32" r:id="rId6"/>
-    <hyperlink ref="J33" r:id="rId7"/>
-    <hyperlink ref="J34" r:id="rId8" display="https://gismaps.osu.edu/arcgis/rest/services/OSUMaps/Transportation/MapServer/23"/>
-    <hyperlink ref="J35" r:id="rId9"/>
-    <hyperlink ref="J23" r:id="rId10"/>
-    <hyperlink ref="J24" r:id="rId11"/>
-    <hyperlink ref="J25" r:id="rId12"/>
-    <hyperlink ref="J20" r:id="rId13"/>
-    <hyperlink ref="J18" r:id="rId14"/>
-    <hyperlink ref="J16" r:id="rId15"/>
-    <hyperlink ref="J11" r:id="rId16"/>
+    <hyperlink ref="J35" r:id="rId2"/>
+    <hyperlink ref="J28" r:id="rId3"/>
+    <hyperlink ref="J29" r:id="rId4"/>
+    <hyperlink ref="J30" r:id="rId5"/>
+    <hyperlink ref="J31" r:id="rId6"/>
+    <hyperlink ref="J32" r:id="rId7"/>
+    <hyperlink ref="J33" r:id="rId8" display="https://gismaps.osu.edu/arcgis/rest/services/OSUMaps/Transportation/MapServer/23"/>
+    <hyperlink ref="J34" r:id="rId9"/>
+    <hyperlink ref="J22" r:id="rId10"/>
+    <hyperlink ref="J23" r:id="rId11"/>
+    <hyperlink ref="J24" r:id="rId12"/>
+    <hyperlink ref="J19" r:id="rId13"/>
+    <hyperlink ref="J17" r:id="rId14"/>
+    <hyperlink ref="J15" r:id="rId15"/>
+    <hyperlink ref="J10" r:id="rId16"/>
     <hyperlink ref="J8" r:id="rId17"/>
     <hyperlink ref="J9" r:id="rId18"/>
-    <hyperlink ref="J10" r:id="rId19"/>
-    <hyperlink ref="J7" r:id="rId20"/>
-    <hyperlink ref="J4" r:id="rId21"/>
+    <hyperlink ref="J7" r:id="rId19"/>
+    <hyperlink ref="J4" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -2261,7 +2225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add some functions about bounds
</commit_message>
<xml_diff>
--- a/layerInventory.xlsx
+++ b/layerInventory.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="174">
   <si>
     <t>mapID</t>
   </si>
@@ -537,6 +537,12 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>dataType</t>
+  </si>
+  <si>
+    <t>layerType</t>
   </si>
 </sst>
 </file>
@@ -875,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,11 +894,11 @@
     <col min="3" max="5" width="25.85546875" hidden="1" customWidth="1"/>
     <col min="6" max="11" width="25.85546875" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="94.140625" customWidth="1"/>
+    <col min="13" max="13" width="94.140625" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -911,6 +917,12 @@
       <c r="F1" t="s">
         <v>160</v>
       </c>
+      <c r="G1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" t="s">
+        <v>172</v>
+      </c>
       <c r="I1" t="s">
         <v>95</v>
       </c>
@@ -926,8 +938,11 @@
       <c r="M1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -967,8 +982,11 @@
       <c r="M2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1008,8 +1026,11 @@
       <c r="M3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1049,8 +1070,11 @@
       <c r="M4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1090,8 +1114,11 @@
       <c r="M5" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1131,8 +1158,11 @@
       <c r="M6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1172,8 +1202,11 @@
       <c r="M7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1213,8 +1246,11 @@
       <c r="M8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1254,8 +1290,11 @@
       <c r="M9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1295,8 +1334,11 @@
       <c r="M10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1336,8 +1378,11 @@
       <c r="M11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1377,8 +1422,11 @@
       <c r="M12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1418,8 +1466,11 @@
       <c r="M13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1459,8 +1510,11 @@
       <c r="M14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1500,8 +1554,11 @@
       <c r="M15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1541,8 +1598,11 @@
       <c r="M16" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1582,8 +1642,11 @@
       <c r="M17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1623,8 +1686,11 @@
       <c r="M18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1664,8 +1730,11 @@
       <c r="M19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1705,8 +1774,11 @@
       <c r="M20" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1746,8 +1818,11 @@
       <c r="M21" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1787,8 +1862,11 @@
       <c r="M22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1828,8 +1906,11 @@
       <c r="M23" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1869,8 +1950,11 @@
       <c r="M24" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1910,8 +1994,11 @@
       <c r="M25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1951,8 +2038,11 @@
       <c r="M26" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1992,8 +2082,11 @@
       <c r="M27" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2033,8 +2126,11 @@
       <c r="M28" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -2074,8 +2170,11 @@
       <c r="M29" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2115,8 +2214,11 @@
       <c r="M30" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2156,8 +2258,11 @@
       <c r="M31" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2197,8 +2302,11 @@
       <c r="M32" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -2238,8 +2346,11 @@
       <c r="M33" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2279,8 +2390,11 @@
       <c r="M34" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2320,8 +2434,11 @@
       <c r="M35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
Add default feature layer addhandle and air_coal &air_ngp
</commit_message>
<xml_diff>
--- a/layerInventory.xlsx
+++ b/layerInventory.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="172">
   <si>
     <t>mapID</t>
   </si>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,10 +1034,10 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -1078,10 +1078,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
@@ -2467,6 +2467,9 @@
       </c>
       <c r="L36" t="s">
         <v>110</v>
+      </c>
+      <c r="M36" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>